<commit_message>
Nice dynamic checkbox example
</commit_message>
<xml_diff>
--- a/CheckboxExample.xlsx
+++ b/CheckboxExample.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biegertm\OneDrive - Starkey\Desktop\Toss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C5308EC-BA35-401F-9550-5DEB7296231D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A8BEE-5E21-4BD1-B2EE-DDED26364BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63405" yWindow="150" windowWidth="21600" windowHeight="12675" xr2:uid="{C1A831B0-67FD-46D8-9CAD-021AAAA9F66F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C1A831B0-67FD-46D8-9CAD-021AAAA9F66F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Initial" sheetId="1" r:id="rId1"/>
+    <sheet name="Dynamic" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dynamic!$A$5:$F$49</definedName>
+    <definedName name="Check_Percent">_xlfn.LAMBDA(_xlpm.x,SUM(--_xlpm.x)/SUM(--NOT(ISBLANK(_xlpm.x))))</definedName>
+    <definedName name="rng">Dynamic!$A$3:$A$20</definedName>
+    <definedName name="rng_status">Dynamic!$B$3:$B$20</definedName>
+    <definedName name="rng_used">INDEX(rng,1):INDEX(rng,COUNT(rng),)</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -53,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Progress</t>
   </si>
@@ -93,12 +101,51 @@
   <si>
     <t>https://www.youtube.com/watch?v=nqfQQVoHT-4</t>
   </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>Item 3</t>
+  </si>
+  <si>
+    <t>Item 4</t>
+  </si>
+  <si>
+    <t>Item 5</t>
+  </si>
+  <si>
+    <t>Item 6</t>
+  </si>
+  <si>
+    <t>Item 7</t>
+  </si>
+  <si>
+    <t>Item 8</t>
+  </si>
+  <si>
+    <t>Item 9</t>
+  </si>
+  <si>
+    <t>Item 10</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=";;;"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,20 +161,102 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000099"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -144,22 +273,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="11">
+    <cellStyle name="20% - Accent1 2" xfId="10" xr:uid="{9C3B6AAC-8FD5-4F3B-B112-04F13DC79A10}"/>
+    <cellStyle name="20% - Accent3 2" xfId="3" xr:uid="{3B25CDBE-2454-4D63-A2EB-C85EC7AD9548}"/>
+    <cellStyle name="Comment" xfId="7" xr:uid="{1ED6F7D8-385A-46EB-8DAA-9CEF79C7C95D}"/>
+    <cellStyle name="Explanatory Text 2" xfId="5" xr:uid="{E32C7E26-4B85-4B7B-9591-1331326F923E}"/>
+    <cellStyle name="Heading 1 2" xfId="4" xr:uid="{3CF68AA6-3418-4C61-9D4D-5DBC49767832}"/>
+    <cellStyle name="Heading 2 2" xfId="9" xr:uid="{30797999-9E7D-43F5-BB89-ECD1F4A18278}"/>
+    <cellStyle name="Heading 3 2" xfId="8" xr:uid="{28575135-C25A-4F95-B638-CB3DE4A3DF75}"/>
+    <cellStyle name="Input 2" xfId="6" xr:uid="{D5C7C395-4498-4B35-9A04-0A3C56AB2026}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{8287760D-7FE6-45E4-BE66-EB0DAB6D507B}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <top style="double">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Biegert Standard" table="0" count="4" xr9:uid="{7ACB024E-3649-4CA6-94E1-0CDA5E6658D5}">
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="totalRow" dxfId="6"/>
+      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+    </tableStyle>
+    <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{14892D05-8A8B-4026-B05E-D5F459195937}">
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="totalRow" dxfId="2"/>
+      <tableStyleElement type="firstColumn" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -172,11 +439,47 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B7" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$F$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -203,6 +506,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$12" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B3" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -210,15 +517,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>148591</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>567690</xdr:colOff>
+          <xdr:colOff>571500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>11431</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -274,14 +581,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>148863</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="295275" cy="226695"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
@@ -290,7 +602,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88AC25B9-C169-4019-8F58-EE477DDC0B6B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -330,20 +642,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>149135</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="295275" cy="226695"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
@@ -352,7 +669,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F997C800-C836-4FCA-AAAC-378038C77F51}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -392,20 +709,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>149407</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="295275" cy="226695"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
@@ -414,7 +736,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2355CF69-7EFE-4CD2-ACAD-B528A463A9DC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -454,20 +776,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>149679</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="295275" cy="226695"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
@@ -476,7 +803,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C747EC7-36A9-43A8-AC40-E95D648C28C3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -516,20 +843,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>149951</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="295275" cy="226695"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
@@ -538,7 +870,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1365F8F-50E2-40DA-9B9C-EA7A4B8F420E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -578,20 +910,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>150223</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="295275" cy="226695"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
@@ -600,7 +937,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EDA212F-08BE-4B69-8BA5-565554EBBE43}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -640,20 +977,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>268605</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>148591</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="295275" cy="226695"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
@@ -662,7 +1004,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B47EC3-E7A2-4BE3-BA5F-141429CA6F13}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -702,6 +1044,636 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEBA56C-3E60-4E8D-86F4-B989C75E5D46}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E15CB4C7-E21D-4B6F-B4B0-261CB908C85D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2052" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65E5D26F-9097-4465-9EA8-D65CAB35209B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2053"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAD57C65-E62D-41B7-8110-30815EFF98F6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B384F657-5EE8-4AB2-B666-26CCD38680A9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2055" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DAEA505-56F5-47F7-B21C-5C59CC1F22F0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2056" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2056"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DF3640B-FE62-41E1-B481-83B55F7475C3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2057" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2057"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBC0133-FF52-4F24-92DE-990C86315D8A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2058" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69350C49-17FF-402B-81A4-0AF4B50093AC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
       </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
@@ -710,9 +1682,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -750,7 +1722,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -856,7 +1828,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -998,7 +1970,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1008,22 +1980,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC56EE99-6C6A-4B7A-AC05-EDB5D06C846E}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1034,32 +2006,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" cm="1">
         <f t="array" ref="C4">SUM(--F5:F12)/COUNT(--F5:F12)</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1067,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1075,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1083,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1091,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1099,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1109,6 +2081,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9575C865-34B9-477D-9F74-94396429DC81}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -1118,18 +2102,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{00FD558C-5806-41ED-9030-5C1FB0066439}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9575C865-34B9-477D-9F74-94396429DC81}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1155,7 +2127,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>571500</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1175,9 +2147,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1197,9 +2169,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1219,9 +2191,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1241,9 +2213,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1263,9 +2235,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1285,9 +2257,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1307,9 +2279,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:colOff>561975</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1323,14 +2295,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{00FD558C-5806-41ED-9030-5C1FB0066439}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
           <x14:cfRule type="dataBar" id="{9575C865-34B9-477D-9F74-94396429DC81}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -1343,10 +2307,1015 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{00FD558C-5806-41ED-9030-5C1FB0066439}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD4F848-6105-4D0E-B180-CA6C72A01336}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="10.7109375" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" cm="1">
+        <f t="array" ref="B1">Check_Percent(rng_status)</f>
+        <v>0.7</v>
+      </c>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>IF(ISBLANK(B3),"",SUM(A2,1))</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A20" si="0">IF(ISBLANK(B4),"",SUM(A3,1))</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+    </row>
+    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+    </row>
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+    </row>
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+    </row>
+    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+    </row>
+    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+    </row>
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+    </row>
+    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId4" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2050" r:id="rId5" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2051" r:id="rId6" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2052" r:id="rId7" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2053" r:id="rId8" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2054" r:id="rId9" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2055" r:id="rId10" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2056" r:id="rId11" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2057" r:id="rId12" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2058" r:id="rId13" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot to test with extention
</commit_message>
<xml_diff>
--- a/CheckboxExample.xlsx
+++ b/CheckboxExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A8BEE-5E21-4BD1-B2EE-DDED26364BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDC163F-F273-431C-A9F8-51A456807F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C1A831B0-67FD-46D8-9CAD-021AAAA9F66F}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Progress</t>
   </si>
@@ -137,6 +137,12 @@
   <si>
     <t>Status</t>
   </si>
+  <si>
+    <t>Item 11</t>
+  </si>
+  <si>
+    <t>Item 12</t>
+  </si>
 </sst>
 </file>
 
@@ -145,7 +151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,11 +224,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -443,11 +444,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,11 +456,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,8 +479,16 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B12" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B13" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,7 +516,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1122,14 +1131,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
@@ -1138,7 +1152,7 @@
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEBA56C-3E60-4E8D-86F4-B989C75E5D46}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1178,20 +1192,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
@@ -1200,7 +1219,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E15CB4C7-E21D-4B6F-B4B0-261CB908C85D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1240,20 +1259,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2052" name="Check Box 4" hidden="1">
@@ -1262,7 +1286,7 @@
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65E5D26F-9097-4465-9EA8-D65CAB35209B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1302,20 +1326,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
@@ -1324,7 +1353,7 @@
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAD57C65-E62D-41B7-8110-30815EFF98F6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1364,20 +1393,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
@@ -1386,7 +1420,7 @@
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B384F657-5EE8-4AB2-B666-26CCD38680A9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1426,20 +1460,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2055" name="Check Box 7" hidden="1">
@@ -1448,7 +1487,7 @@
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DAEA505-56F5-47F7-B21C-5C59CC1F22F0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1488,20 +1527,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2056" name="Check Box 8" hidden="1">
@@ -1510,7 +1554,7 @@
                   <a14:compatExt spid="_x0000_s2056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DF3640B-FE62-41E1-B481-83B55F7475C3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1550,20 +1594,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2057" name="Check Box 9" hidden="1">
@@ -1572,7 +1621,7 @@
                   <a14:compatExt spid="_x0000_s2057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBC0133-FF52-4F24-92DE-990C86315D8A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1612,6 +1661,135 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2058" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="304800" cy="219075"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2059" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2059"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE92CD14-38B0-4E13-83C4-6CB92B3FEA81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
       </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
@@ -1622,19 +1800,19 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>12</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:ext cx="304800" cy="219075"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2058" name="Check Box 10" hidden="1">
+            <xdr:cNvPr id="2060" name="Check Box 12" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2058"/>
+                  <a14:compatExt spid="_x0000_s2060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69350C49-17FF-402B-81A4-0AF4B50093AC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6368B748-CB04-4B39-A022-7A52C7F78C92}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2328,7 +2506,7 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2520,7 @@
       </c>
       <c r="B1" cm="1">
         <f t="array" ref="B1">Check_Percent(rng_status)</f>
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -2373,7 +2551,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2392,7 +2570,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -2411,7 +2589,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -2449,7 +2627,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -2468,7 +2646,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -2558,12 +2736,16 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
+      <c r="A13">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -2573,12 +2755,16 @@
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
+      <c r="A14">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
@@ -3314,6 +3500,50 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2059" r:id="rId14" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2060" r:id="rId15" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>

<commit_message>
Added graphic for status
</commit_message>
<xml_diff>
--- a/CheckboxExample.xlsx
+++ b/CheckboxExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biegertm\OneDrive - Starkey Hearing Technologies\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DC3987-5CCB-42C5-9CC5-364E1948F8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B730A6FC-F9EA-448D-B5E5-0ABD861AB342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C1A831B0-67FD-46D8-9CAD-021AAAA9F66F}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{C1A831B0-67FD-46D8-9CAD-021AAAA9F66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dynamic!$A$5:$F$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dynamic!$A$6:$F$50</definedName>
     <definedName name="Check_Percent">_xlfn.LAMBDA(_xlpm.x,SUM(--_xlpm.x)/SUM(--NOT(ISBLANK(_xlpm.x))))</definedName>
-    <definedName name="rng">Dynamic!$A$3:$A$20</definedName>
-    <definedName name="rng_status">Dynamic!$B$3:$B$20</definedName>
+    <definedName name="rng">Dynamic!$A$4:$A$21</definedName>
+    <definedName name="rng_status">Dynamic!$B$4:$B$21</definedName>
     <definedName name="rng_used">INDEX(rng,1):INDEX(rng,COUNT(rng),)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Progress</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>2-D check box example</t>
+  </si>
+  <si>
+    <t>Blank</t>
   </si>
 </sst>
 </file>
@@ -251,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,12 +281,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,7 +347,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -481,48 +478,781 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15293545693151994"/>
+          <c:y val="7.9207893347229941E-2"/>
+          <c:w val="0.69412908613696012"/>
+          <c:h val="0.80638070515121574"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6ED6-449E-93E8-B36E737F08B6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-6ED6-449E-93E8-B36E737F08B6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>Dynamic!$B$1:$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.41666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58333333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6ED6-449E-93E8-B36E737F08B6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="90"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$F$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,7 +1260,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="B14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -558,7 +1288,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="B4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1110,13 +1840,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>1</xdr:row>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>3</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1177,13 +1907,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>2</xdr:row>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1244,13 +1974,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>3</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1311,13 +2041,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>6</xdr:row>
+          <xdr:row>7</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1378,13 +2108,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>7</xdr:row>
+          <xdr:row>8</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1445,13 +2175,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>6</xdr:row>
+          <xdr:row>7</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1512,13 +2242,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>7</xdr:row>
+          <xdr:row>8</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1579,13 +2309,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1646,13 +2376,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>12</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1713,13 +2443,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1780,13 +2510,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>12</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>13</xdr:row>
+          <xdr:row>14</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1847,13 +2577,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>542925</xdr:colOff>
-          <xdr:row>14</xdr:row>
+          <xdr:row>15</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1908,13 +2638,125 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{454291DE-C70D-29EC-98E9-B73EA437ABBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="$B$2">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B28E19D-575D-3815-0803-8C597E44D982}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3362325" y="619125"/>
+          <a:ext cx="666750" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{79B63F60-6AA6-45EC-9C04-9E5B39BE6712}" type="TxLink">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>58%</a:t>
+          </a:fld>
+          <a:endParaRPr lang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1952,7 +2794,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2058,7 +2900,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2200,7 +3042,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2555,10 +3397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD4F848-6105-4D0E-B180-CA6C72A01336}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2566,28 +3408,23 @@
     <col min="1" max="16384" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" cm="1">
-        <f t="array" ref="B1">Check_Percent(rng_status)</f>
-        <v>0.75</v>
-      </c>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3">
+        <f>1-B2</f>
+        <v>0.41666666666666663</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2"/>
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" cm="1">
+        <f t="array" ref="B2">Check_Percent(rng_status)</f>
+        <v>0.58333333333333337</v>
+      </c>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
@@ -2598,16 +3435,11 @@
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>IF(ISBLANK(B3),"",SUM(A2,1))</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -2618,14 +3450,14 @@
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A20" si="0">IF(ISBLANK(B4),"",SUM(A3,1))</f>
-        <v>2</v>
+        <f>IF(ISBLANK(B4),"",SUM(A3,1))</f>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
@@ -2637,14 +3469,14 @@
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="A5:A21" si="0">IF(ISBLANK(B5),"",SUM(A4,1))</f>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -2657,13 +3489,13 @@
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -2676,13 +3508,13 @@
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -2695,13 +3527,13 @@
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
@@ -2714,13 +3546,13 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -2733,13 +3565,13 @@
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -2752,13 +3584,13 @@
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -2771,13 +3603,13 @@
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -2790,13 +3622,13 @@
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -2809,13 +3641,13 @@
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -2826,12 +3658,16 @@
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
+      <c r="A15">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
@@ -2916,8 +3752,11 @@
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B21" s="4"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
@@ -3322,6 +4161,18 @@
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
+    </row>
+    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -3335,28 +4186,6 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="2049" r:id="rId4" name="Check Box 1">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>238125</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>542925</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId5" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3378,7 +4207,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2051" r:id="rId6" name="Check Box 3">
+            <control shapeId="2050" r:id="rId5" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3400,7 +4229,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2052" r:id="rId7" name="Check Box 4">
+            <control shapeId="2051" r:id="rId6" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3422,7 +4251,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2053" r:id="rId8" name="Check Box 5">
+            <control shapeId="2052" r:id="rId7" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3444,7 +4273,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2054" r:id="rId9" name="Check Box 6">
+            <control shapeId="2053" r:id="rId8" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3466,7 +4295,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2055" r:id="rId10" name="Check Box 7">
+            <control shapeId="2054" r:id="rId9" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3488,7 +4317,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2056" r:id="rId11" name="Check Box 8">
+            <control shapeId="2055" r:id="rId10" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3510,7 +4339,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2057" r:id="rId12" name="Check Box 9">
+            <control shapeId="2056" r:id="rId11" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3532,7 +4361,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2058" r:id="rId13" name="Check Box 10">
+            <control shapeId="2057" r:id="rId12" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3554,7 +4383,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2059" r:id="rId14" name="Check Box 11">
+            <control shapeId="2058" r:id="rId13" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3576,7 +4405,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2060" r:id="rId15" name="Check Box 12">
+            <control shapeId="2059" r:id="rId14" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3596,6 +4425,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2060" r:id="rId15" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
@@ -3606,7 +4457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AE38F2-25EB-4F6F-8FFA-7E7FDE260297}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added note on line chart progress illustration
</commit_message>
<xml_diff>
--- a/CheckboxExample.xlsx
+++ b/CheckboxExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B730A6FC-F9EA-448D-B5E5-0ABD861AB342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCC5313-CBBD-42CC-B9D2-B238F9969300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{C1A831B0-67FD-46D8-9CAD-021AAAA9F66F}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{C1A831B0-67FD-46D8-9CAD-021AAAA9F66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Progress</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Blank</t>
+  </si>
+  <si>
+    <t>I have created a workbook with a need line chart that illustrates discreet milestones.</t>
   </si>
 </sst>
 </file>
@@ -650,565 +653,6 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2656,7 +2100,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{454291DE-C70D-29EC-98E9-B73EA437ABBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2136,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B28E19D-575D-3815-0803-8C597E44D982}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3400,7 +2844,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3684,7 +3128,9 @@
       <c r="B16" s="4"/>
       <c r="C16"/>
       <c r="D16"/>
-      <c r="E16"/>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
@@ -3692,10 +3138,6 @@
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="B17" s="4"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -3708,7 +3150,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(B18),"",SUM(E16,1))</f>
         <v/>
       </c>
       <c r="B18" s="4"/>

</xml_diff>